<commit_message>
update excel function to write raw csv data
</commit_message>
<xml_diff>
--- a/output/excel/HVAC BOQ - Ducting.xlsx
+++ b/output/excel/HVAC BOQ - Ducting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Preston.Padayachee\Git\CoDe.Hackathon\PARKpy\output\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{89C63B3F-D4DF-4A82-9B0F-16B6B17A9E70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1DC9353D-87E1-41E2-9B94-5C653247303D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="10152" xr2:uid="{5E9FBE50-8C1B-4B87-8DA2-869D6687090D}"/>
+    <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="10152" xr2:uid="{0DE680D8-53D4-4D7D-B728-52BCF7AB5FB0}"/>
   </bookViews>
   <sheets>
     <sheet name="MainBOQ" sheetId="2" r:id="rId1"/>
@@ -379,7 +379,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C5794F2-BA6E-46A4-B139-51AB68F41F8E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0CBE3A3-A94C-4DD2-A017-0C6AD81CB626}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
update excel function to save raw csv data
</commit_message>
<xml_diff>
--- a/output/excel/HVAC BOQ - Ducting.xlsx
+++ b/output/excel/HVAC BOQ - Ducting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Preston.Padayachee\Git\CoDe.Hackathon\PARKpy\output\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1DC9353D-87E1-41E2-9B94-5C653247303D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4DE72E-C18D-46F0-8B2B-DF2E3F51FA94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="10152" xr2:uid="{0DE680D8-53D4-4D7D-B728-52BCF7AB5FB0}"/>
+    <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="10152" xr2:uid="{19613CE6-3F22-4E89-B376-985B46244221}"/>
   </bookViews>
   <sheets>
     <sheet name="MainBOQ" sheetId="2" r:id="rId1"/>
@@ -31,6 +31,53 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="14">
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Rate</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Section</t>
+  </si>
+  <si>
+    <t>BOQ_Duct Fitting Schedule Low Pressure Insulated Cladded Rect</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>BOQ_Duct Fitting Schedule Low Pressure Insulated Rect</t>
+  </si>
+  <si>
+    <t>BOQ_Duct Fitting Schedule Medium Pressure Insulated Cladded Rect</t>
+  </si>
+  <si>
+    <t>BOQ_Duct Fitting Schedule Medium Pressure Insulated Rect</t>
+  </si>
+  <si>
+    <t>BOQ_Duct Schedule Low Pressure Insulated Cladded Rect</t>
+  </si>
+  <si>
+    <t>BOQ_Duct Schedule Low Pressure Insulated Rect</t>
+  </si>
+  <si>
+    <t>BOQ_Duct Schedule Medium Pressure Insulated Cladded Rect</t>
+  </si>
+  <si>
+    <t>BOQ_Duct Schedule Medium Pressure Insulated Rect</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -379,13 +426,603 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0CBE3A3-A94C-4DD2-A017-0C6AD81CB626}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35708DA1-7B4F-4AE7-A853-B5FE87E68A38}">
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>80.412999999999997</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>80.412999999999997</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>56.749000000000002</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>226.99600000000001</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>7.9169999999999998</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>39.585000000000001</v>
+      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>346.99400000000003</v>
+      </c>
+      <c r="F5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>191.64</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>191.64</v>
+      </c>
+      <c r="F6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>23.481000000000002</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>93.924000000000007</v>
+      </c>
+      <c r="F7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>12.795999999999999</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>63.98</v>
+      </c>
+      <c r="F8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9">
+        <v>349.54400000000004</v>
+      </c>
+      <c r="F9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>2.2250000000000001</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>2.2250000000000001</v>
+      </c>
+      <c r="F10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>50.07</v>
+      </c>
+      <c r="D11">
+        <v>2.5</v>
+      </c>
+      <c r="E11">
+        <v>125.175</v>
+      </c>
+      <c r="F11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>55.371000000000002</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <v>221.48400000000001</v>
+      </c>
+      <c r="F12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13">
+        <v>348.88400000000001</v>
+      </c>
+      <c r="F13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>43.420999999999999</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>43.420999999999999</v>
+      </c>
+      <c r="F14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>29.355</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="E15">
+        <v>117.42</v>
+      </c>
+      <c r="F15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16">
+        <v>160.84100000000001</v>
+      </c>
+      <c r="F16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>257.459</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>257.459</v>
+      </c>
+      <c r="F17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>38.450000000000003</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+      <c r="E18">
+        <v>153.80000000000001</v>
+      </c>
+      <c r="F18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>3.9460000000000002</v>
+      </c>
+      <c r="D19">
+        <v>5</v>
+      </c>
+      <c r="E19">
+        <v>19.73</v>
+      </c>
+      <c r="F19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20">
+        <v>430.98899999999998</v>
+      </c>
+      <c r="F20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>0</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>1284.5530000000001</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>1284.5530000000001</v>
+      </c>
+      <c r="F21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>220.42599999999999</v>
+      </c>
+      <c r="D22">
+        <v>4</v>
+      </c>
+      <c r="E22">
+        <v>881.70399999999995</v>
+      </c>
+      <c r="F22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23">
+        <v>119.98699999999999</v>
+      </c>
+      <c r="D23">
+        <v>5</v>
+      </c>
+      <c r="E23">
+        <v>599.93499999999995</v>
+      </c>
+      <c r="F23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24">
+        <v>2766.192</v>
+      </c>
+      <c r="F24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>0</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>3.0680000000000001</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>3.0680000000000001</v>
+      </c>
+      <c r="F25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>40.884</v>
+      </c>
+      <c r="D26">
+        <v>2.5</v>
+      </c>
+      <c r="E26">
+        <v>102.21</v>
+      </c>
+      <c r="F26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>2</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27">
+        <v>18.408000000000001</v>
+      </c>
+      <c r="D27">
+        <v>4</v>
+      </c>
+      <c r="E27">
+        <v>73.632000000000005</v>
+      </c>
+      <c r="F27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>3</v>
+      </c>
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28">
+        <v>178.91000000000005</v>
+      </c>
+      <c r="F28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>0</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>92.774000000000001</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>92.774000000000001</v>
+      </c>
+      <c r="F29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <v>65.975999999999999</v>
+      </c>
+      <c r="D30">
+        <v>4</v>
+      </c>
+      <c r="E30">
+        <v>263.904</v>
+      </c>
+      <c r="F30" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>2</v>
+      </c>
+      <c r="B31">
+        <v>4</v>
+      </c>
+      <c r="C31">
+        <v>19.332000000000001</v>
+      </c>
+      <c r="D31">
+        <v>5</v>
+      </c>
+      <c r="E31">
+        <v>96.66</v>
+      </c>
+      <c r="F31" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>3</v>
+      </c>
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32">
+        <v>453.33800000000002</v>
+      </c>
+      <c r="F32" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix excel output and unittest run(path error)
</commit_message>
<xml_diff>
--- a/output/excel/HVAC BOQ - Ducting.xlsx
+++ b/output/excel/HVAC BOQ - Ducting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Preston.Padayachee\Git\CoDe.Hackathon\PARKpy\output\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A758CB1A-9326-4B7A-85D4-3F8E734B74F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA9E211E-B6CA-4B93-9CA8-0C325222D5D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1464" yWindow="1464" windowWidth="17280" windowHeight="10152" xr2:uid="{9771A922-0217-4770-8C99-7F95B405EF55}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="10152" xr2:uid="{24BEFD19-FE09-456D-8C04-0597FAB93FA8}"/>
   </bookViews>
   <sheets>
     <sheet name="MainBOQ" sheetId="2" r:id="rId1"/>
@@ -423,7 +423,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{587C1090-2514-49C6-ABDF-913654D2C261}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79825982-BDCB-45C9-8C27-7CD6C6AB68FC}">
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
initialise excel output formatting
</commit_message>
<xml_diff>
--- a/output/excel/HVAC BOQ - Ducting.xlsx
+++ b/output/excel/HVAC BOQ - Ducting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Preston.Padayachee\Git\CoDe.Hackathon\PARKpy\output\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA9E211E-B6CA-4B93-9CA8-0C325222D5D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98D11210-E81A-444D-AE97-64B0998F54BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="10152" xr2:uid="{24BEFD19-FE09-456D-8C04-0597FAB93FA8}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="10152" xr2:uid="{1B125915-7AF4-42B0-9F62-AF7FDD0C3C09}"/>
   </bookViews>
   <sheets>
     <sheet name="MainBOQ" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="21">
   <si>
     <t>Item</t>
   </si>
@@ -72,7 +72,31 @@
     <t>Category 5 (2100&lt;W or 2100&lt;H)</t>
   </si>
   <si>
-    <t>m²</t>
+    <t>BOQ_Duct Fitting Schedule Low Pressure Insulated Cladded Rect</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>BOQ_Duct Fitting Schedule Low Pressure Insulated Rect</t>
+  </si>
+  <si>
+    <t>BOQ_Duct Fitting Schedule Medium Pressure Insulated Cladded Rect</t>
+  </si>
+  <si>
+    <t>BOQ_Duct Fitting Schedule Medium Pressure Insulated Rect</t>
+  </si>
+  <si>
+    <t>BOQ_Duct Schedule Low Pressure Insulated Cladded Rect</t>
+  </si>
+  <si>
+    <t>BOQ_Duct Schedule Low Pressure Insulated Rect</t>
+  </si>
+  <si>
+    <t>BOQ_Duct Schedule Medium Pressure Insulated Cladded Rect</t>
+  </si>
+  <si>
+    <t>BOQ_Duct Schedule Medium Pressure Insulated Rect</t>
   </si>
 </sst>
 </file>
@@ -423,8 +447,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79825982-BDCB-45C9-8C27-7CD6C6AB68FC}">
-  <dimension ref="A1:F8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D470103-3DE8-4A2F-92CC-FEB9AFEF7464}">
+  <dimension ref="A1:G64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -432,13 +456,14 @@
   <cols>
     <col min="1" max="1" width="4.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="57.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -458,7 +483,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -466,67 +491,76 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1.1000000000000001</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>80.412999999999997</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>80.412999999999997</v>
+      </c>
+      <c r="G3" t="s">
         <v>12</v>
       </c>
-      <c r="D3">
-        <v>1955.5530000000001</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1955.5530000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1.2</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>56.749000000000002</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>226.99600000000001</v>
+      </c>
+      <c r="G4" t="s">
         <v>12</v>
       </c>
-      <c r="D4">
-        <v>90.954000000000008</v>
-      </c>
-      <c r="E4">
-        <v>2.5</v>
-      </c>
-      <c r="F4">
-        <v>227.38499999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1.3</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>7.9169999999999998</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>39.585000000000001</v>
+      </c>
+      <c r="G5" t="s">
         <v>12</v>
       </c>
-      <c r="D5">
-        <v>508.21600000000001</v>
-      </c>
-      <c r="E5">
-        <v>4</v>
-      </c>
-      <c r="F5">
-        <v>2032.864</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1.4</v>
       </c>
@@ -534,29 +568,915 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6">
+        <v>346.99400000000003</v>
+      </c>
+      <c r="G6" t="s">
         <v>12</v>
       </c>
-      <c r="D6">
-        <v>163.97799999999998</v>
-      </c>
-      <c r="E6">
-        <v>5</v>
-      </c>
-      <c r="F6">
-        <v>819.88999999999987</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1.5</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>191.64</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>191.64</v>
+      </c>
+      <c r="G7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>23.481000000000002</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
       <c r="F8">
         <v>5035.6919999999991</v>
+      </c>
+      <c r="G8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>12.795999999999999</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>63.98</v>
+      </c>
+      <c r="G9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10">
+        <v>349.54400000000004</v>
+      </c>
+      <c r="G10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>2.2250000000000001</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>2.2250000000000001</v>
+      </c>
+      <c r="G11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>50.07</v>
+      </c>
+      <c r="E12">
+        <v>2.5</v>
+      </c>
+      <c r="F12">
+        <v>125.175</v>
+      </c>
+      <c r="G12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>55.371000000000002</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <v>221.48400000000001</v>
+      </c>
+      <c r="G13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14">
+        <v>348.88400000000001</v>
+      </c>
+      <c r="G14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>43.420999999999999</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>43.420999999999999</v>
+      </c>
+      <c r="G15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>29.355</v>
+      </c>
+      <c r="E16">
+        <v>4</v>
+      </c>
+      <c r="F16">
+        <v>117.42</v>
+      </c>
+      <c r="G16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17">
+        <v>160.84100000000001</v>
+      </c>
+      <c r="G17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>257.459</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>257.459</v>
+      </c>
+      <c r="G18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <v>38.450000000000003</v>
+      </c>
+      <c r="E19">
+        <v>4</v>
+      </c>
+      <c r="F19">
+        <v>153.80000000000001</v>
+      </c>
+      <c r="G19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="D20">
+        <v>3.9460000000000002</v>
+      </c>
+      <c r="E20">
+        <v>5</v>
+      </c>
+      <c r="F20">
+        <v>19.73</v>
+      </c>
+      <c r="G20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21">
+        <v>430.98899999999998</v>
+      </c>
+      <c r="G21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>1284.5530000000001</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>1284.5530000000001</v>
+      </c>
+      <c r="G22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>220.42599999999999</v>
+      </c>
+      <c r="E23">
+        <v>4</v>
+      </c>
+      <c r="F23">
+        <v>881.70399999999995</v>
+      </c>
+      <c r="G23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24">
+        <v>119.98699999999999</v>
+      </c>
+      <c r="E24">
+        <v>5</v>
+      </c>
+      <c r="F24">
+        <v>599.93499999999995</v>
+      </c>
+      <c r="G24" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25">
+        <v>2766.192</v>
+      </c>
+      <c r="G25" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>3.0680000000000001</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>3.0680000000000001</v>
+      </c>
+      <c r="G26" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27">
+        <v>40.884</v>
+      </c>
+      <c r="E27">
+        <v>2.5</v>
+      </c>
+      <c r="F27">
+        <v>102.21</v>
+      </c>
+      <c r="G27" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C28">
+        <v>3</v>
+      </c>
+      <c r="D28">
+        <v>18.408000000000001</v>
+      </c>
+      <c r="E28">
+        <v>4</v>
+      </c>
+      <c r="F28">
+        <v>73.632000000000005</v>
+      </c>
+      <c r="G28" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C29" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29">
+        <v>178.91000000000005</v>
+      </c>
+      <c r="G29" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>92.774000000000001</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>92.774000000000001</v>
+      </c>
+      <c r="G30" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C31">
+        <v>3</v>
+      </c>
+      <c r="D31">
+        <v>65.975999999999999</v>
+      </c>
+      <c r="E31">
+        <v>4</v>
+      </c>
+      <c r="F31">
+        <v>263.904</v>
+      </c>
+      <c r="G31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C32">
+        <v>4</v>
+      </c>
+      <c r="D32">
+        <v>19.332000000000001</v>
+      </c>
+      <c r="E32">
+        <v>5</v>
+      </c>
+      <c r="F32">
+        <v>96.66</v>
+      </c>
+      <c r="G32" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33">
+        <v>453.33800000000002</v>
+      </c>
+      <c r="G33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>80.412999999999997</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>80.412999999999997</v>
+      </c>
+      <c r="G34" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C35">
+        <v>3</v>
+      </c>
+      <c r="D35">
+        <v>56.749000000000002</v>
+      </c>
+      <c r="E35">
+        <v>4</v>
+      </c>
+      <c r="F35">
+        <v>226.99600000000001</v>
+      </c>
+      <c r="G35" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C36">
+        <v>4</v>
+      </c>
+      <c r="D36">
+        <v>7.9169999999999998</v>
+      </c>
+      <c r="E36">
+        <v>5</v>
+      </c>
+      <c r="F36">
+        <v>39.585000000000001</v>
+      </c>
+      <c r="G36" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C37" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37">
+        <v>346.99400000000003</v>
+      </c>
+      <c r="G37" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>191.64</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38">
+        <v>191.64</v>
+      </c>
+      <c r="G38" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C39">
+        <v>3</v>
+      </c>
+      <c r="D39">
+        <v>23.481000000000002</v>
+      </c>
+      <c r="E39">
+        <v>4</v>
+      </c>
+      <c r="F39">
+        <v>93.924000000000007</v>
+      </c>
+      <c r="G39" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C40">
+        <v>4</v>
+      </c>
+      <c r="D40">
+        <v>12.795999999999999</v>
+      </c>
+      <c r="E40">
+        <v>5</v>
+      </c>
+      <c r="F40">
+        <v>63.98</v>
+      </c>
+      <c r="G40" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C41" t="s">
+        <v>13</v>
+      </c>
+      <c r="F41">
+        <v>349.54400000000004</v>
+      </c>
+      <c r="G41" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>2.2250000000000001</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42">
+        <v>2.2250000000000001</v>
+      </c>
+      <c r="G42" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C43">
+        <v>2</v>
+      </c>
+      <c r="D43">
+        <v>50.07</v>
+      </c>
+      <c r="E43">
+        <v>2.5</v>
+      </c>
+      <c r="F43">
+        <v>125.175</v>
+      </c>
+      <c r="G43" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C44">
+        <v>3</v>
+      </c>
+      <c r="D44">
+        <v>55.371000000000002</v>
+      </c>
+      <c r="E44">
+        <v>4</v>
+      </c>
+      <c r="F44">
+        <v>221.48400000000001</v>
+      </c>
+      <c r="G44" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C45" t="s">
+        <v>13</v>
+      </c>
+      <c r="F45">
+        <v>348.88400000000001</v>
+      </c>
+      <c r="G45" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>43.420999999999999</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46">
+        <v>43.420999999999999</v>
+      </c>
+      <c r="G46" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C47">
+        <v>3</v>
+      </c>
+      <c r="D47">
+        <v>29.355</v>
+      </c>
+      <c r="E47">
+        <v>4</v>
+      </c>
+      <c r="F47">
+        <v>117.42</v>
+      </c>
+      <c r="G47" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C48" t="s">
+        <v>13</v>
+      </c>
+      <c r="F48">
+        <v>160.84100000000001</v>
+      </c>
+      <c r="G48" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>257.459</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49">
+        <v>257.459</v>
+      </c>
+      <c r="G49" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C50">
+        <v>3</v>
+      </c>
+      <c r="D50">
+        <v>38.450000000000003</v>
+      </c>
+      <c r="E50">
+        <v>4</v>
+      </c>
+      <c r="F50">
+        <v>153.80000000000001</v>
+      </c>
+      <c r="G50" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C51">
+        <v>4</v>
+      </c>
+      <c r="D51">
+        <v>3.9460000000000002</v>
+      </c>
+      <c r="E51">
+        <v>5</v>
+      </c>
+      <c r="F51">
+        <v>19.73</v>
+      </c>
+      <c r="G51" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C52" t="s">
+        <v>13</v>
+      </c>
+      <c r="F52">
+        <v>430.98899999999998</v>
+      </c>
+      <c r="G52" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="53" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53">
+        <v>1284.5530000000001</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53">
+        <v>1284.5530000000001</v>
+      </c>
+      <c r="G53" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="54" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C54">
+        <v>3</v>
+      </c>
+      <c r="D54">
+        <v>220.42599999999999</v>
+      </c>
+      <c r="E54">
+        <v>4</v>
+      </c>
+      <c r="F54">
+        <v>881.70399999999995</v>
+      </c>
+      <c r="G54" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="55" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C55">
+        <v>4</v>
+      </c>
+      <c r="D55">
+        <v>119.98699999999999</v>
+      </c>
+      <c r="E55">
+        <v>5</v>
+      </c>
+      <c r="F55">
+        <v>599.93499999999995</v>
+      </c>
+      <c r="G55" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="56" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C56" t="s">
+        <v>13</v>
+      </c>
+      <c r="F56">
+        <v>2766.192</v>
+      </c>
+      <c r="G56" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="57" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <v>3.0680000000000001</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="F57">
+        <v>3.0680000000000001</v>
+      </c>
+      <c r="G57" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="58" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C58">
+        <v>2</v>
+      </c>
+      <c r="D58">
+        <v>40.884</v>
+      </c>
+      <c r="E58">
+        <v>2.5</v>
+      </c>
+      <c r="F58">
+        <v>102.21</v>
+      </c>
+      <c r="G58" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="59" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C59">
+        <v>3</v>
+      </c>
+      <c r="D59">
+        <v>18.408000000000001</v>
+      </c>
+      <c r="E59">
+        <v>4</v>
+      </c>
+      <c r="F59">
+        <v>73.632000000000005</v>
+      </c>
+      <c r="G59" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="60" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C60" t="s">
+        <v>13</v>
+      </c>
+      <c r="F60">
+        <v>178.91000000000005</v>
+      </c>
+      <c r="G60" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="61" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C61">
+        <v>1</v>
+      </c>
+      <c r="D61">
+        <v>92.774000000000001</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
+      <c r="F61">
+        <v>92.774000000000001</v>
+      </c>
+      <c r="G61" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="62" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C62">
+        <v>3</v>
+      </c>
+      <c r="D62">
+        <v>65.975999999999999</v>
+      </c>
+      <c r="E62">
+        <v>4</v>
+      </c>
+      <c r="F62">
+        <v>263.904</v>
+      </c>
+      <c r="G62" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="63" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C63">
+        <v>4</v>
+      </c>
+      <c r="D63">
+        <v>19.332000000000001</v>
+      </c>
+      <c r="E63">
+        <v>5</v>
+      </c>
+      <c r="F63">
+        <v>96.66</v>
+      </c>
+      <c r="G63" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="64" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C64" t="s">
+        <v>13</v>
+      </c>
+      <c r="F64">
+        <v>453.33800000000002</v>
+      </c>
+      <c r="G64" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added create excel sheet function
</commit_message>
<xml_diff>
--- a/output/excel/HVAC BOQ - Ducting.xlsx
+++ b/output/excel/HVAC BOQ - Ducting.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Preston.Padayachee\Git\CoDe.Hackathon\PARKpy\output\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98D11210-E81A-444D-AE97-64B0998F54BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35F4D95F-4D84-4CE9-A62D-A4AC27CC1D53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="10152" xr2:uid="{1B125915-7AF4-42B0-9F62-AF7FDD0C3C09}"/>
+    <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="10152" xr2:uid="{42A8C747-33C5-4A18-AA7F-BCA04953069F}"/>
   </bookViews>
   <sheets>
-    <sheet name="MainBOQ" sheetId="2" r:id="rId1"/>
+    <sheet name="Summary" sheetId="3" r:id="rId1"/>
+    <sheet name="Main_BOQ" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,34 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="21">
+  <si>
+    <t>BOQ_Duct Fitting Schedule Low Pressure Insulated Cladded Rect</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>BOQ_Duct Fitting Schedule Low Pressure Insulated Rect</t>
+  </si>
+  <si>
+    <t>BOQ_Duct Fitting Schedule Medium Pressure Insulated Cladded Rect</t>
+  </si>
+  <si>
+    <t>BOQ_Duct Fitting Schedule Medium Pressure Insulated Rect</t>
+  </si>
+  <si>
+    <t>BOQ_Duct Schedule Low Pressure Insulated Cladded Rect</t>
+  </si>
+  <si>
+    <t>BOQ_Duct Schedule Low Pressure Insulated Rect</t>
+  </si>
+  <si>
+    <t>BOQ_Duct Schedule Medium Pressure Insulated Cladded Rect</t>
+  </si>
+  <si>
+    <t>BOQ_Duct Schedule Medium Pressure Insulated Rect</t>
+  </si>
   <si>
     <t>Item</t>
   </si>
@@ -70,33 +99,6 @@
   </si>
   <si>
     <t>Category 5 (2100&lt;W or 2100&lt;H)</t>
-  </si>
-  <si>
-    <t>BOQ_Duct Fitting Schedule Low Pressure Insulated Cladded Rect</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>BOQ_Duct Fitting Schedule Low Pressure Insulated Rect</t>
-  </si>
-  <si>
-    <t>BOQ_Duct Fitting Schedule Medium Pressure Insulated Cladded Rect</t>
-  </si>
-  <si>
-    <t>BOQ_Duct Fitting Schedule Medium Pressure Insulated Rect</t>
-  </si>
-  <si>
-    <t>BOQ_Duct Schedule Low Pressure Insulated Cladded Rect</t>
-  </si>
-  <si>
-    <t>BOQ_Duct Schedule Low Pressure Insulated Rect</t>
-  </si>
-  <si>
-    <t>BOQ_Duct Schedule Medium Pressure Insulated Cladded Rect</t>
-  </si>
-  <si>
-    <t>BOQ_Duct Schedule Medium Pressure Insulated Rect</t>
   </si>
 </sst>
 </file>
@@ -447,40 +449,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D470103-3DE8-4A2F-92CC-FEB9AFEF7464}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CB419E2-E38B-46AF-A326-2F7A9C39663A}">
   <dimension ref="A1:G64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="57.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="57.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -488,7 +488,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>15</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>226.99600000000001</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -496,7 +505,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -511,7 +520,7 @@
         <v>80.412999999999997</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -519,7 +528,7 @@
         <v>1.2</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -534,7 +543,7 @@
         <v>226.99600000000001</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -542,7 +551,7 @@
         <v>1.3</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -557,7 +566,7 @@
         <v>39.585000000000001</v>
       </c>
       <c r="G5" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -565,16 +574,16 @@
         <v>1.4</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="F6">
         <v>346.99400000000003</v>
       </c>
       <c r="G6" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -582,7 +591,7 @@
         <v>1.5</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -597,10 +606,13 @@
         <v>191.64</v>
       </c>
       <c r="G7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
       <c r="C8">
         <v>3</v>
       </c>
@@ -614,10 +626,16 @@
         <v>5035.6919999999991</v>
       </c>
       <c r="G8" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>2.2250000000000001</v>
+      </c>
       <c r="C9">
         <v>4</v>
       </c>
@@ -631,21 +649,33 @@
         <v>63.98</v>
       </c>
       <c r="G9" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>50.07</v>
+      </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="F10">
         <v>349.54400000000004</v>
       </c>
       <c r="G10" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>55.371000000000002</v>
+      </c>
       <c r="C11">
         <v>1</v>
       </c>
@@ -659,10 +689,13 @@
         <v>2.2250000000000001</v>
       </c>
       <c r="G11" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
       <c r="C12">
         <v>2</v>
       </c>
@@ -676,10 +709,16 @@
         <v>125.175</v>
       </c>
       <c r="G12" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>43.420999999999999</v>
+      </c>
       <c r="C13">
         <v>3</v>
       </c>
@@ -693,21 +732,30 @@
         <v>221.48400000000001</v>
       </c>
       <c r="G13" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <v>29.355</v>
+      </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="F14">
         <v>348.88400000000001</v>
       </c>
       <c r="G14" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
       <c r="C15">
         <v>1</v>
       </c>
@@ -721,10 +769,16 @@
         <v>43.420999999999999</v>
       </c>
       <c r="G15" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>257.459</v>
+      </c>
       <c r="C16">
         <v>3</v>
       </c>
@@ -738,21 +792,33 @@
         <v>117.42</v>
       </c>
       <c r="G16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>3</v>
+      </c>
+      <c r="B17">
+        <v>38.450000000000003</v>
+      </c>
       <c r="C17" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="F17">
         <v>160.84100000000001</v>
       </c>
       <c r="G17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>4</v>
+      </c>
+      <c r="B18">
+        <v>3.9460000000000002</v>
+      </c>
       <c r="C18">
         <v>1</v>
       </c>
@@ -766,10 +832,13 @@
         <v>257.459</v>
       </c>
       <c r="G18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
       <c r="C19">
         <v>3</v>
       </c>
@@ -783,10 +852,16 @@
         <v>153.80000000000001</v>
       </c>
       <c r="G19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>1284.5530000000001</v>
+      </c>
       <c r="C20">
         <v>4</v>
       </c>
@@ -800,21 +875,33 @@
         <v>19.73</v>
       </c>
       <c r="G20" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>3</v>
+      </c>
+      <c r="B21">
+        <v>220.42599999999999</v>
+      </c>
       <c r="C21" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="F21">
         <v>430.98899999999998</v>
       </c>
       <c r="G21" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>4</v>
+      </c>
+      <c r="B22">
+        <v>119.98699999999999</v>
+      </c>
       <c r="C22">
         <v>1</v>
       </c>
@@ -828,10 +915,13 @@
         <v>1284.5530000000001</v>
       </c>
       <c r="G22" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>1</v>
+      </c>
       <c r="C23">
         <v>3</v>
       </c>
@@ -845,10 +935,16 @@
         <v>881.70399999999995</v>
       </c>
       <c r="G23" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <v>3.0680000000000001</v>
+      </c>
       <c r="C24">
         <v>4</v>
       </c>
@@ -862,21 +958,33 @@
         <v>599.93499999999995</v>
       </c>
       <c r="G24" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="B25">
+        <v>40.884</v>
+      </c>
       <c r="C25" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="F25">
         <v>2766.192</v>
       </c>
       <c r="G25" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>3</v>
+      </c>
+      <c r="B26">
+        <v>18.408000000000001</v>
+      </c>
       <c r="C26">
         <v>1</v>
       </c>
@@ -890,10 +998,13 @@
         <v>3.0680000000000001</v>
       </c>
       <c r="G26" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>1</v>
+      </c>
       <c r="C27">
         <v>2</v>
       </c>
@@ -907,10 +1018,16 @@
         <v>102.21</v>
       </c>
       <c r="G27" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28">
+        <v>92.774000000000001</v>
+      </c>
       <c r="C28">
         <v>3</v>
       </c>
@@ -924,21 +1041,33 @@
         <v>73.632000000000005</v>
       </c>
       <c r="G28" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>3</v>
+      </c>
+      <c r="B29">
+        <v>65.975999999999999</v>
+      </c>
       <c r="C29" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="F29">
         <v>178.91000000000005</v>
       </c>
       <c r="G29" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>4</v>
+      </c>
+      <c r="B30">
+        <v>19.332000000000001</v>
+      </c>
       <c r="C30">
         <v>1</v>
       </c>
@@ -952,10 +1081,13 @@
         <v>92.774000000000001</v>
       </c>
       <c r="G30" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>1</v>
+      </c>
       <c r="C31">
         <v>3</v>
       </c>
@@ -969,10 +1101,16 @@
         <v>263.904</v>
       </c>
       <c r="G31" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32">
+        <v>80.412999999999997</v>
+      </c>
       <c r="C32">
         <v>4</v>
       </c>
@@ -986,21 +1124,33 @@
         <v>96.66</v>
       </c>
       <c r="G32" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>3</v>
+      </c>
+      <c r="B33">
+        <v>56.749000000000002</v>
+      </c>
       <c r="C33" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="F33">
         <v>453.33800000000002</v>
       </c>
       <c r="G33" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>4</v>
+      </c>
+      <c r="B34">
+        <v>7.9169999999999998</v>
+      </c>
       <c r="C34">
         <v>1</v>
       </c>
@@ -1014,10 +1164,13 @@
         <v>80.412999999999997</v>
       </c>
       <c r="G34" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>1</v>
+      </c>
       <c r="C35">
         <v>3</v>
       </c>
@@ -1031,10 +1184,16 @@
         <v>226.99600000000001</v>
       </c>
       <c r="G35" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36">
+        <v>191.64</v>
+      </c>
       <c r="C36">
         <v>4</v>
       </c>
@@ -1048,21 +1207,33 @@
         <v>39.585000000000001</v>
       </c>
       <c r="G36" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>3</v>
+      </c>
+      <c r="B37">
+        <v>23.481000000000002</v>
+      </c>
       <c r="C37" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="F37">
         <v>346.99400000000003</v>
       </c>
       <c r="G37" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>4</v>
+      </c>
+      <c r="B38">
+        <v>12.795999999999999</v>
+      </c>
       <c r="C38">
         <v>1</v>
       </c>
@@ -1076,10 +1247,13 @@
         <v>191.64</v>
       </c>
       <c r="G38" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="39" spans="3:7" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>1</v>
+      </c>
       <c r="C39">
         <v>3</v>
       </c>
@@ -1093,10 +1267,16 @@
         <v>93.924000000000007</v>
       </c>
       <c r="G39" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="40" spans="3:7" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="B40">
+        <v>2.2250000000000001</v>
+      </c>
       <c r="C40">
         <v>4</v>
       </c>
@@ -1110,21 +1290,33 @@
         <v>63.98</v>
       </c>
       <c r="G40" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>2</v>
+      </c>
+      <c r="B41">
+        <v>50.07</v>
+      </c>
       <c r="C41" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="F41">
         <v>349.54400000000004</v>
       </c>
       <c r="G41" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="42" spans="3:7" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>3</v>
+      </c>
+      <c r="B42">
+        <v>55.371000000000002</v>
+      </c>
       <c r="C42">
         <v>1</v>
       </c>
@@ -1138,10 +1330,13 @@
         <v>2.2250000000000001</v>
       </c>
       <c r="G42" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="43" spans="3:7" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>1</v>
+      </c>
       <c r="C43">
         <v>2</v>
       </c>
@@ -1155,10 +1350,16 @@
         <v>125.175</v>
       </c>
       <c r="G43" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="44" spans="3:7" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>1</v>
+      </c>
+      <c r="B44">
+        <v>43.420999999999999</v>
+      </c>
       <c r="C44">
         <v>3</v>
       </c>
@@ -1172,21 +1373,30 @@
         <v>221.48400000000001</v>
       </c>
       <c r="G44" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="45" spans="3:7" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>3</v>
+      </c>
+      <c r="B45">
+        <v>29.355</v>
+      </c>
       <c r="C45" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="F45">
         <v>348.88400000000001</v>
       </c>
       <c r="G45" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="46" spans="3:7" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>1</v>
+      </c>
       <c r="C46">
         <v>1</v>
       </c>
@@ -1200,10 +1410,16 @@
         <v>43.420999999999999</v>
       </c>
       <c r="G46" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="47" spans="3:7" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>1</v>
+      </c>
+      <c r="B47">
+        <v>257.459</v>
+      </c>
       <c r="C47">
         <v>3</v>
       </c>
@@ -1217,21 +1433,33 @@
         <v>117.42</v>
       </c>
       <c r="G47" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="48" spans="3:7" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>3</v>
+      </c>
+      <c r="B48">
+        <v>38.450000000000003</v>
+      </c>
       <c r="C48" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="F48">
         <v>160.84100000000001</v>
       </c>
       <c r="G48" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="49" spans="3:7" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>4</v>
+      </c>
+      <c r="B49">
+        <v>3.9460000000000002</v>
+      </c>
       <c r="C49">
         <v>1</v>
       </c>
@@ -1245,10 +1473,13 @@
         <v>257.459</v>
       </c>
       <c r="G49" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="50" spans="3:7" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>1</v>
+      </c>
       <c r="C50">
         <v>3</v>
       </c>
@@ -1262,10 +1493,16 @@
         <v>153.80000000000001</v>
       </c>
       <c r="G50" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="51" spans="3:7" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>1</v>
+      </c>
+      <c r="B51">
+        <v>1284.5530000000001</v>
+      </c>
       <c r="C51">
         <v>4</v>
       </c>
@@ -1279,21 +1516,33 @@
         <v>19.73</v>
       </c>
       <c r="G51" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="52" spans="3:7" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>3</v>
+      </c>
+      <c r="B52">
+        <v>220.42599999999999</v>
+      </c>
       <c r="C52" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="F52">
         <v>430.98899999999998</v>
       </c>
       <c r="G52" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="53" spans="3:7" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>4</v>
+      </c>
+      <c r="B53">
+        <v>119.98699999999999</v>
+      </c>
       <c r="C53">
         <v>1</v>
       </c>
@@ -1307,10 +1556,13 @@
         <v>1284.5530000000001</v>
       </c>
       <c r="G53" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="54" spans="3:7" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>1</v>
+      </c>
       <c r="C54">
         <v>3</v>
       </c>
@@ -1324,10 +1576,16 @@
         <v>881.70399999999995</v>
       </c>
       <c r="G54" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="55" spans="3:7" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>1</v>
+      </c>
+      <c r="B55">
+        <v>3.0680000000000001</v>
+      </c>
       <c r="C55">
         <v>4</v>
       </c>
@@ -1341,21 +1599,33 @@
         <v>599.93499999999995</v>
       </c>
       <c r="G55" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="56" spans="3:7" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>2</v>
+      </c>
+      <c r="B56">
+        <v>40.884</v>
+      </c>
       <c r="C56" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="F56">
         <v>2766.192</v>
       </c>
       <c r="G56" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="57" spans="3:7" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>3</v>
+      </c>
+      <c r="B57">
+        <v>18.408000000000001</v>
+      </c>
       <c r="C57">
         <v>1</v>
       </c>
@@ -1369,10 +1639,13 @@
         <v>3.0680000000000001</v>
       </c>
       <c r="G57" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="58" spans="3:7" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>1</v>
+      </c>
       <c r="C58">
         <v>2</v>
       </c>
@@ -1386,10 +1659,16 @@
         <v>102.21</v>
       </c>
       <c r="G58" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="59" spans="3:7" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>1</v>
+      </c>
+      <c r="B59">
+        <v>92.774000000000001</v>
+      </c>
       <c r="C59">
         <v>3</v>
       </c>
@@ -1403,21 +1682,33 @@
         <v>73.632000000000005</v>
       </c>
       <c r="G59" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="60" spans="3:7" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>3</v>
+      </c>
+      <c r="B60">
+        <v>65.975999999999999</v>
+      </c>
       <c r="C60" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="F60">
         <v>178.91000000000005</v>
       </c>
       <c r="G60" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="61" spans="3:7" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>4</v>
+      </c>
+      <c r="B61">
+        <v>19.332000000000001</v>
+      </c>
       <c r="C61">
         <v>1</v>
       </c>
@@ -1431,10 +1722,13 @@
         <v>92.774000000000001</v>
       </c>
       <c r="G61" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="62" spans="3:7" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>1</v>
+      </c>
       <c r="C62">
         <v>3</v>
       </c>
@@ -1448,10 +1742,10 @@
         <v>263.904</v>
       </c>
       <c r="G62" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="63" spans="3:7" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C63">
         <v>4</v>
       </c>
@@ -1465,21 +1759,1011 @@
         <v>96.66</v>
       </c>
       <c r="G63" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="64" spans="3:7" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C64" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="F64">
         <v>453.33800000000002</v>
       </c>
       <c r="G64" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48CFDEE5-78BF-42E2-BB48-3395132D53A5}">
+  <dimension ref="A1:E62"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="57.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>80.412999999999997</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>80.412999999999997</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>56.749000000000002</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>226.99600000000001</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>7.9169999999999998</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>39.585000000000001</v>
+      </c>
+      <c r="E3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>346.99400000000003</v>
+      </c>
+      <c r="E4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>191.64</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>191.64</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>23.481000000000002</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>93.924000000000007</v>
+      </c>
+      <c r="E6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>12.795999999999999</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>63.98</v>
+      </c>
+      <c r="E7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>349.54400000000004</v>
+      </c>
+      <c r="E8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>2.2250000000000001</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>2.2250000000000001</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>50.07</v>
+      </c>
+      <c r="C10">
+        <v>2.5</v>
+      </c>
+      <c r="D10">
+        <v>125.175</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>55.371000000000002</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>221.48400000000001</v>
+      </c>
+      <c r="E11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>348.88400000000001</v>
+      </c>
+      <c r="E12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>43.420999999999999</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>43.420999999999999</v>
+      </c>
+      <c r="E13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <v>29.355</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
+      </c>
+      <c r="D14">
+        <v>117.42</v>
+      </c>
+      <c r="E14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>160.84100000000001</v>
+      </c>
+      <c r="E15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>257.459</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>257.459</v>
+      </c>
+      <c r="E16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>3</v>
+      </c>
+      <c r="B17">
+        <v>38.450000000000003</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <v>153.80000000000001</v>
+      </c>
+      <c r="E17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>4</v>
+      </c>
+      <c r="B18">
+        <v>3.9460000000000002</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
+      </c>
+      <c r="D18">
+        <v>19.73</v>
+      </c>
+      <c r="E18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>430.98899999999998</v>
+      </c>
+      <c r="E19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>1284.5530000000001</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1284.5530000000001</v>
+      </c>
+      <c r="E20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>3</v>
+      </c>
+      <c r="B21">
+        <v>220.42599999999999</v>
+      </c>
+      <c r="C21">
+        <v>4</v>
+      </c>
+      <c r="D21">
+        <v>881.70399999999995</v>
+      </c>
+      <c r="E21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>4</v>
+      </c>
+      <c r="B22">
+        <v>119.98699999999999</v>
+      </c>
+      <c r="C22">
+        <v>5</v>
+      </c>
+      <c r="D22">
+        <v>599.93499999999995</v>
+      </c>
+      <c r="E22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>2766.192</v>
+      </c>
+      <c r="E23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <v>3.0680000000000001</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>3.0680000000000001</v>
+      </c>
+      <c r="E24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="B25">
+        <v>40.884</v>
+      </c>
+      <c r="C25">
+        <v>2.5</v>
+      </c>
+      <c r="D25">
+        <v>102.21</v>
+      </c>
+      <c r="E25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>3</v>
+      </c>
+      <c r="B26">
+        <v>18.408000000000001</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="D26">
+        <v>73.632000000000005</v>
+      </c>
+      <c r="E26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>178.91000000000005</v>
+      </c>
+      <c r="E27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28">
+        <v>92.774000000000001</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>92.774000000000001</v>
+      </c>
+      <c r="E28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>3</v>
+      </c>
+      <c r="B29">
+        <v>65.975999999999999</v>
+      </c>
+      <c r="C29">
+        <v>4</v>
+      </c>
+      <c r="D29">
+        <v>263.904</v>
+      </c>
+      <c r="E29" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>4</v>
+      </c>
+      <c r="B30">
+        <v>19.332000000000001</v>
+      </c>
+      <c r="C30">
+        <v>5</v>
+      </c>
+      <c r="D30">
+        <v>96.66</v>
+      </c>
+      <c r="E30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>453.33800000000002</v>
+      </c>
+      <c r="E31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32">
+        <v>80.412999999999997</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>80.412999999999997</v>
+      </c>
+      <c r="E32" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>3</v>
+      </c>
+      <c r="B33">
+        <v>56.749000000000002</v>
+      </c>
+      <c r="C33">
+        <v>4</v>
+      </c>
+      <c r="D33">
+        <v>226.99600000000001</v>
+      </c>
+      <c r="E33" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>4</v>
+      </c>
+      <c r="B34">
+        <v>7.9169999999999998</v>
+      </c>
+      <c r="C34">
+        <v>5</v>
+      </c>
+      <c r="D34">
+        <v>39.585000000000001</v>
+      </c>
+      <c r="E34" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>346.99400000000003</v>
+      </c>
+      <c r="E35" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36">
+        <v>191.64</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>191.64</v>
+      </c>
+      <c r="E36" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>3</v>
+      </c>
+      <c r="B37">
+        <v>23.481000000000002</v>
+      </c>
+      <c r="C37">
+        <v>4</v>
+      </c>
+      <c r="D37">
+        <v>93.924000000000007</v>
+      </c>
+      <c r="E37" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>4</v>
+      </c>
+      <c r="B38">
+        <v>12.795999999999999</v>
+      </c>
+      <c r="C38">
+        <v>5</v>
+      </c>
+      <c r="D38">
+        <v>63.98</v>
+      </c>
+      <c r="E38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>349.54400000000004</v>
+      </c>
+      <c r="E39" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="B40">
+        <v>2.2250000000000001</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>2.2250000000000001</v>
+      </c>
+      <c r="E40" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>2</v>
+      </c>
+      <c r="B41">
+        <v>50.07</v>
+      </c>
+      <c r="C41">
+        <v>2.5</v>
+      </c>
+      <c r="D41">
+        <v>125.175</v>
+      </c>
+      <c r="E41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>3</v>
+      </c>
+      <c r="B42">
+        <v>55.371000000000002</v>
+      </c>
+      <c r="C42">
+        <v>4</v>
+      </c>
+      <c r="D42">
+        <v>221.48400000000001</v>
+      </c>
+      <c r="E42" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>348.88400000000001</v>
+      </c>
+      <c r="E43" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>1</v>
+      </c>
+      <c r="B44">
+        <v>43.420999999999999</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>43.420999999999999</v>
+      </c>
+      <c r="E44" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>3</v>
+      </c>
+      <c r="B45">
+        <v>29.355</v>
+      </c>
+      <c r="C45">
+        <v>4</v>
+      </c>
+      <c r="D45">
+        <v>117.42</v>
+      </c>
+      <c r="E45" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>160.84100000000001</v>
+      </c>
+      <c r="E46" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>1</v>
+      </c>
+      <c r="B47">
+        <v>257.459</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>257.459</v>
+      </c>
+      <c r="E47" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>3</v>
+      </c>
+      <c r="B48">
+        <v>38.450000000000003</v>
+      </c>
+      <c r="C48">
+        <v>4</v>
+      </c>
+      <c r="D48">
+        <v>153.80000000000001</v>
+      </c>
+      <c r="E48" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>4</v>
+      </c>
+      <c r="B49">
+        <v>3.9460000000000002</v>
+      </c>
+      <c r="C49">
+        <v>5</v>
+      </c>
+      <c r="D49">
+        <v>19.73</v>
+      </c>
+      <c r="E49" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>430.98899999999998</v>
+      </c>
+      <c r="E50" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>1</v>
+      </c>
+      <c r="B51">
+        <v>1284.5530000000001</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>1284.5530000000001</v>
+      </c>
+      <c r="E51" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>3</v>
+      </c>
+      <c r="B52">
+        <v>220.42599999999999</v>
+      </c>
+      <c r="C52">
+        <v>4</v>
+      </c>
+      <c r="D52">
+        <v>881.70399999999995</v>
+      </c>
+      <c r="E52" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>4</v>
+      </c>
+      <c r="B53">
+        <v>119.98699999999999</v>
+      </c>
+      <c r="C53">
+        <v>5</v>
+      </c>
+      <c r="D53">
+        <v>599.93499999999995</v>
+      </c>
+      <c r="E53" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>2766.192</v>
+      </c>
+      <c r="E54" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>1</v>
+      </c>
+      <c r="B55">
+        <v>3.0680000000000001</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55">
+        <v>3.0680000000000001</v>
+      </c>
+      <c r="E55" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>2</v>
+      </c>
+      <c r="B56">
+        <v>40.884</v>
+      </c>
+      <c r="C56">
+        <v>2.5</v>
+      </c>
+      <c r="D56">
+        <v>102.21</v>
+      </c>
+      <c r="E56" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>3</v>
+      </c>
+      <c r="B57">
+        <v>18.408000000000001</v>
+      </c>
+      <c r="C57">
+        <v>4</v>
+      </c>
+      <c r="D57">
+        <v>73.632000000000005</v>
+      </c>
+      <c r="E57" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>1</v>
+      </c>
+      <c r="D58">
+        <v>178.91000000000005</v>
+      </c>
+      <c r="E58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>1</v>
+      </c>
+      <c r="B59">
+        <v>92.774000000000001</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59">
+        <v>92.774000000000001</v>
+      </c>
+      <c r="E59" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>3</v>
+      </c>
+      <c r="B60">
+        <v>65.975999999999999</v>
+      </c>
+      <c r="C60">
+        <v>4</v>
+      </c>
+      <c r="D60">
+        <v>263.904</v>
+      </c>
+      <c r="E60" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>4</v>
+      </c>
+      <c r="B61">
+        <v>19.332000000000001</v>
+      </c>
+      <c r="C61">
+        <v>5</v>
+      </c>
+      <c r="D61">
+        <v>96.66</v>
+      </c>
+      <c r="E61" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>1</v>
+      </c>
+      <c r="D62">
+        <v>453.33800000000002</v>
+      </c>
+      <c r="E62" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B32CC9AA-9D73-4EE6-AE4C-32D73863C24B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>